<commit_message>
[Mod, Add] : String Data에 이벤트 문구 추가, 맵 SkyColor -> Solid Color 로 변경, 맵 씬 카메라 각도 74 -> 60으로 수정
</commit_message>
<xml_diff>
--- a/Assets/10.Data/StringTable.xlsx
+++ b/Assets/10.Data/StringTable.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SourceTree\Project_60Days\Assets\10.Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SourceTree\Project_DEAD.NET\Assets\10.Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68E2E81B-426D-44C1-8878-888DAF984333}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12870"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>인덱스</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -155,13 +156,89 @@
   </si>
   <si>
     <t>Index</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이벤트(도둑맞은 자원)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>STR_NOTE_LOOSE_RESROUCE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이벤트(사막 모래 폭풍)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>STR_NOTE_DESERT_STORM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;color=red&gt; 경고 : 강력한 모래 폭풍이 감지되었습니다. 강제 안전 조율 시스템을 가동합니다. 다음 1턴동안 선체를 이동할 수 없습니다. &lt;/color&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>STR_NOTE_SEARCH_TUNDRA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이벤트(툰드라 구조물 탐색)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이 구조물은 얼어붙어 있다. 탐사에 오랜 시간이 소요될 것 같다.
+(접근 승인 선택 시 1턴 동안 이동 불가 [선택 시점에 이동 불가])</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>STR_NOTE_ACIDENT_ETHER</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이벤트(에테르 가스 수집 중 사고)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;color=red&gt;경고 : 에테르 가스 수집 중 예상치 못한 폭발이 감지되었습니다. 선체 추출 기능이 비활성화되었습니다. 자가 수복 프로토콜을 시작합니다.
+다음 1턴 동안 선체를 이동할 수 없습니다.&lt;/color&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">STR_NOTE_LOOSE_WAY </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이벤트(수풀 속 길잃음)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;color=red&gt; 경고 : 선체의 방향타 시스템에 오류가 발생하였습니다. 이전에 선택한 경로가 아닌 다른 방향으로 이동하였을 가능성이 있습니다.
+선체 위치를 확인, 조정해 주십시오. &lt;/color&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이벤트(늪에 빠짐)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>STR_NOTE_SWAMP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;color=red&gt; 경고 : 선체가 정글의 거대한 늪에 빠졌습니다. 자가 수복 프로토콜을 시작합니다.
+다음 1턴 동안 선체를 이동할 수 없습니다.&lt;/color&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>분석에 따르면 {0}의 보유량이 감소했다고 한다. 소실인가? 혹은 잘못 센 것인가? [{0} 보유량 - 1]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -179,7 +256,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -195,6 +272,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -265,7 +354,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -276,6 +365,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -293,8 +385,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -575,27 +673,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.625" customWidth="1"/>
-    <col min="2" max="2" width="18.875" customWidth="1"/>
+    <col min="2" max="2" width="29.125" customWidth="1"/>
     <col min="3" max="3" width="13.125" customWidth="1"/>
-    <col min="4" max="4" width="21.5" customWidth="1"/>
-    <col min="5" max="5" width="26.75" customWidth="1"/>
+    <col min="4" max="4" width="29.375" customWidth="1"/>
+    <col min="5" max="5" width="83.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="6" t="s">
         <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -607,19 +705,19 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="4" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="4"/>
-      <c r="B2" s="5"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="6"/>
       <c r="C2" s="2" t="s">
         <v>32</v>
       </c>
@@ -640,265 +738,299 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="10">
         <v>1001</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="3">
-        <v>-1</v>
-      </c>
-      <c r="G3" s="3">
-        <v>-1</v>
-      </c>
-      <c r="H3" s="3">
+      <c r="F3" s="10">
+        <v>-1</v>
+      </c>
+      <c r="G3" s="10">
+        <v>-1</v>
+      </c>
+      <c r="H3" s="10">
         <v>-1</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="7"/>
-      <c r="B4" s="3" t="s">
+      <c r="A4" s="8"/>
+      <c r="B4" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="10">
         <v>1002</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="3">
-        <v>-1</v>
-      </c>
-      <c r="G4" s="3">
-        <v>-1</v>
-      </c>
-      <c r="H4" s="3">
+      <c r="F4" s="10">
+        <v>-1</v>
+      </c>
+      <c r="G4" s="10">
+        <v>-1</v>
+      </c>
+      <c r="H4" s="10">
         <v>-1</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="7"/>
-      <c r="B5" s="3" t="s">
+      <c r="A5" s="8"/>
+      <c r="B5" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="10">
         <v>1003</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="3">
-        <v>-1</v>
-      </c>
-      <c r="G5" s="3">
-        <v>-1</v>
-      </c>
-      <c r="H5" s="3">
+      <c r="F5" s="10">
+        <v>-1</v>
+      </c>
+      <c r="G5" s="10">
+        <v>-1</v>
+      </c>
+      <c r="H5" s="10">
         <v>-1</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="7"/>
-      <c r="B6" s="3" t="s">
+      <c r="A6" s="8"/>
+      <c r="B6" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="10">
         <v>1004</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="3">
-        <v>-1</v>
-      </c>
-      <c r="G6" s="3">
-        <v>-1</v>
-      </c>
-      <c r="H6" s="3">
+      <c r="F6" s="10">
+        <v>-1</v>
+      </c>
+      <c r="G6" s="10">
+        <v>-1</v>
+      </c>
+      <c r="H6" s="10">
         <v>-1</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="7"/>
-      <c r="B7" s="3" t="s">
+      <c r="A7" s="8"/>
+      <c r="B7" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="10">
         <v>1005</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="3">
-        <v>-1</v>
-      </c>
-      <c r="G7" s="3">
-        <v>-1</v>
-      </c>
-      <c r="H7" s="3">
+      <c r="F7" s="10">
+        <v>-1</v>
+      </c>
+      <c r="G7" s="10">
+        <v>-1</v>
+      </c>
+      <c r="H7" s="10">
         <v>-1</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="8"/>
-      <c r="B8" s="3" t="s">
+      <c r="A8" s="9"/>
+      <c r="B8" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="10">
         <v>1006</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="F8" s="3">
-        <v>-1</v>
-      </c>
-      <c r="G8" s="3">
-        <v>-1</v>
-      </c>
-      <c r="H8" s="3">
+      <c r="F8" s="10">
+        <v>-1</v>
+      </c>
+      <c r="G8" s="10">
+        <v>-1</v>
+      </c>
+      <c r="H8" s="10">
         <v>-1</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3">
-        <v>1007</v>
-      </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3">
-        <v>-1</v>
-      </c>
-      <c r="G9" s="3">
-        <v>-1</v>
-      </c>
-      <c r="H9" s="3">
+      <c r="B9" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="11">
+        <v>2001</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="F9" s="11">
+        <v>-1</v>
+      </c>
+      <c r="G9" s="11">
+        <v>-1</v>
+      </c>
+      <c r="H9" s="11">
         <v>-1</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3">
-        <v>1008</v>
-      </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3">
-        <v>-1</v>
-      </c>
-      <c r="G10" s="3">
-        <v>-1</v>
-      </c>
-      <c r="H10" s="3">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B10" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="11">
+        <v>2002</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" s="11">
+        <v>-1</v>
+      </c>
+      <c r="G10" s="11">
+        <v>-1</v>
+      </c>
+      <c r="H10" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="33" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3">
-        <v>1009</v>
-      </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3">
-        <v>-1</v>
-      </c>
-      <c r="G11" s="3">
-        <v>-1</v>
-      </c>
-      <c r="H11" s="3">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B11" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="11">
+        <v>2003</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" s="11">
+        <v>-1</v>
+      </c>
+      <c r="G11" s="11">
+        <v>-1</v>
+      </c>
+      <c r="H11" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3">
-        <v>1010</v>
-      </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3">
-        <v>-1</v>
-      </c>
-      <c r="G12" s="3">
-        <v>-1</v>
-      </c>
-      <c r="H12" s="3">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B12" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="11">
+        <v>2004</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" s="11">
+        <v>-1</v>
+      </c>
+      <c r="G12" s="11">
+        <v>-1</v>
+      </c>
+      <c r="H12" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3">
-        <v>1011</v>
-      </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3">
-        <v>-1</v>
-      </c>
-      <c r="G13" s="3">
-        <v>-1</v>
-      </c>
-      <c r="H13" s="3">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B13" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="11">
+        <v>2005</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="11">
+        <v>-1</v>
+      </c>
+      <c r="G13" s="11">
+        <v>-1</v>
+      </c>
+      <c r="H13" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3">
-        <v>1012</v>
-      </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3">
-        <v>-1</v>
-      </c>
-      <c r="G14" s="3">
-        <v>-1</v>
-      </c>
-      <c r="H14" s="3">
+      <c r="B14" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="11">
+        <v>2006</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="F14" s="11">
+        <v>-1</v>
+      </c>
+      <c r="G14" s="11">
+        <v>-1</v>
+      </c>
+      <c r="H14" s="11">
         <v>-1</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
-      <c r="C15" s="3">
-        <v>1013</v>
-      </c>
+      <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3">
@@ -914,9 +1046,7 @@
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
-      <c r="C16" s="3">
-        <v>1014</v>
-      </c>
+      <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3">
@@ -932,9 +1062,7 @@
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
-      <c r="C17" s="3">
-        <v>1015</v>
-      </c>
+      <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3">
@@ -950,9 +1078,7 @@
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
-      <c r="C18" s="3">
-        <v>1016</v>
-      </c>
+      <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3">
@@ -968,9 +1094,7 @@
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
-      <c r="C19" s="3">
-        <v>1017</v>
-      </c>
+      <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3">
@@ -986,9 +1110,7 @@
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
-      <c r="C20" s="3">
-        <v>1018</v>
-      </c>
+      <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
       <c r="F20" s="3">
@@ -1004,9 +1126,7 @@
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
-      <c r="C21" s="3">
-        <v>1019</v>
-      </c>
+      <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
       <c r="F21" s="3">
@@ -1022,9 +1142,7 @@
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
-      <c r="C22" s="3">
-        <v>1020</v>
-      </c>
+      <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3">
@@ -1040,9 +1158,7 @@
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
-      <c r="C23" s="3">
-        <v>1021</v>
-      </c>
+      <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3">
@@ -1058,9 +1174,7 @@
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
-      <c r="C24" s="3">
-        <v>1022</v>
-      </c>
+      <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3">
@@ -1076,9 +1190,7 @@
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
-      <c r="C25" s="3">
-        <v>1023</v>
-      </c>
+      <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3">
@@ -1094,9 +1206,7 @@
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
-      <c r="C26" s="3">
-        <v>1024</v>
-      </c>
+      <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
       <c r="F26" s="3">
@@ -1112,9 +1222,7 @@
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
-      <c r="C27" s="3">
-        <v>1025</v>
-      </c>
+      <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
       <c r="F27" s="3">
@@ -1130,9 +1238,7 @@
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
-      <c r="C28" s="3">
-        <v>1026</v>
-      </c>
+      <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
       <c r="F28" s="3">
@@ -1148,9 +1254,7 @@
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
-      <c r="C29" s="3">
-        <v>1027</v>
-      </c>
+      <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
       <c r="F29" s="3">
@@ -1166,9 +1270,7 @@
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
-      <c r="C30" s="3">
-        <v>1028</v>
-      </c>
+      <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
       <c r="F30" s="3">
@@ -1184,9 +1286,7 @@
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
-      <c r="C31" s="3">
-        <v>1029</v>
-      </c>
+      <c r="C31" s="3"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
       <c r="F31" s="3">
@@ -1202,9 +1302,7 @@
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
-      <c r="C32" s="3">
-        <v>1030</v>
-      </c>
+      <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
       <c r="F32" s="3">
@@ -1220,9 +1318,7 @@
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
-      <c r="C33" s="3">
-        <v>1031</v>
-      </c>
+      <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
       <c r="F33" s="3">

</xml_diff>

<commit_message>
[Add] : 알림/경고 메세지 string data 추가
</commit_message>
<xml_diff>
--- a/Assets/10.Data/StringTable.xlsx
+++ b/Assets/10.Data/StringTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SourceTree\Project_DEAD.NET\Assets\10.Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A549C379-ABF1-4F9C-8DA0-00F437BD185D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1DB608C-23E1-43B0-8B02-438FAB62B6F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20115" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
   <si>
     <t>인덱스</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -284,6 +284,30 @@
   <si>
     <t>툰드라
 얼어붙은 문 : 구조물 탐사 시 2턴 소모</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>알림(알림 사항 있음)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>STR_NEW_NOTICE_ALERT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>새로운 알림이 있습니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>알림(주변 1타일 글리처 경고)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>STR_WARNING_NOTICE_ALERT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>경고 : 주변 1타일 이내에 글리처가 있습니다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -308,7 +332,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -342,6 +366,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -412,7 +442,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -437,6 +467,12 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -452,11 +488,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -741,7 +774,7 @@
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -754,10 +787,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="11" t="s">
         <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -780,8 +813,8 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="8"/>
-      <c r="B2" s="9"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="11"/>
       <c r="C2" s="2" t="s">
         <v>32</v>
       </c>
@@ -802,7 +835,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="12" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -828,7 +861,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="11"/>
+      <c r="A4" s="13"/>
       <c r="B4" s="5" t="s">
         <v>7</v>
       </c>
@@ -852,7 +885,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="11"/>
+      <c r="A5" s="13"/>
       <c r="B5" s="5" t="s">
         <v>8</v>
       </c>
@@ -876,7 +909,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="11"/>
+      <c r="A6" s="13"/>
       <c r="B6" s="5" t="s">
         <v>9</v>
       </c>
@@ -900,7 +933,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="11"/>
+      <c r="A7" s="13"/>
       <c r="B7" s="5" t="s">
         <v>10</v>
       </c>
@@ -924,7 +957,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="12"/>
+      <c r="A8" s="14"/>
       <c r="B8" s="5" t="s">
         <v>15</v>
       </c>
@@ -1093,129 +1126,145 @@
     </row>
     <row r="15" spans="1:8" ht="33" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="C15" s="13">
+      <c r="C15" s="8">
         <v>3001</v>
       </c>
-      <c r="D15" s="13" t="s">
+      <c r="D15" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="E15" s="14" t="s">
+      <c r="E15" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="F15" s="13">
-        <v>-1</v>
-      </c>
-      <c r="G15" s="13">
-        <v>-1</v>
-      </c>
-      <c r="H15" s="13">
+      <c r="F15" s="8">
+        <v>-1</v>
+      </c>
+      <c r="G15" s="8">
+        <v>-1</v>
+      </c>
+      <c r="H15" s="8">
         <v>-1</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="33" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="C16" s="13">
+      <c r="C16" s="8">
         <v>3002</v>
       </c>
-      <c r="D16" s="13" t="s">
+      <c r="D16" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="E16" s="14" t="s">
+      <c r="E16" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="F16" s="13">
-        <v>-1</v>
-      </c>
-      <c r="G16" s="13">
-        <v>-1</v>
-      </c>
-      <c r="H16" s="13">
+      <c r="F16" s="8">
+        <v>-1</v>
+      </c>
+      <c r="G16" s="8">
+        <v>-1</v>
+      </c>
+      <c r="H16" s="8">
         <v>-1</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="33" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="C17" s="13">
+      <c r="C17" s="8">
         <v>3003</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="D17" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="E17" s="14" t="s">
+      <c r="E17" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="F17" s="13">
-        <v>-1</v>
-      </c>
-      <c r="G17" s="13">
-        <v>-1</v>
-      </c>
-      <c r="H17" s="13">
+      <c r="F17" s="8">
+        <v>-1</v>
+      </c>
+      <c r="G17" s="8">
+        <v>-1</v>
+      </c>
+      <c r="H17" s="8">
         <v>-1</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="33" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="C18" s="13">
+      <c r="C18" s="8">
         <v>3004</v>
       </c>
-      <c r="D18" s="13" t="s">
+      <c r="D18" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="E18" s="14" t="s">
+      <c r="E18" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="F18" s="13">
-        <v>-1</v>
-      </c>
-      <c r="G18" s="13">
-        <v>-1</v>
-      </c>
-      <c r="H18" s="13">
+      <c r="F18" s="8">
+        <v>-1</v>
+      </c>
+      <c r="G18" s="8">
+        <v>-1</v>
+      </c>
+      <c r="H18" s="8">
         <v>-1</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3">
-        <v>-1</v>
-      </c>
-      <c r="G19" s="3">
-        <v>-1</v>
-      </c>
-      <c r="H19" s="3">
+      <c r="B19" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" s="15">
+        <v>4001</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="F19" s="15">
+        <v>-1</v>
+      </c>
+      <c r="G19" s="15">
+        <v>-1</v>
+      </c>
+      <c r="H19" s="15">
         <v>-1</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3">
-        <v>-1</v>
-      </c>
-      <c r="G20" s="3">
-        <v>-1</v>
-      </c>
-      <c r="H20" s="3">
+      <c r="B20" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="C20" s="15">
+        <v>4002</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="F20" s="15">
+        <v>-1</v>
+      </c>
+      <c r="G20" s="15">
+        <v>-1</v>
+      </c>
+      <c r="H20" s="15">
         <v>-1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Mod]: Quest 알고리즘 수정
</commit_message>
<xml_diff>
--- a/Assets/10.Data/StringTable.xlsx
+++ b/Assets/10.Data/StringTable.xlsx
@@ -19,12 +19,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="98">
-  <x:si>
-    <x:t>STR_SELECT_JUSTOUDA_KEY</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Justo</x:t>
+<x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="118">
+  <x:si>
+    <x:t>생존 프로세스: 도망</x:t>
   </x:si>
   <x:si>
     <x:t>&lt;color=red&gt; 경고 : 강력한 모래 폭풍이 감지되었습니다. 강제 안전 조율 시스템을 가동합니다. 다음 1턴동안 선체를 이동할 수 없습니다. &lt;/color&gt;</x:t>
@@ -34,214 +31,316 @@
 다음 1턴 동안 선체를 이동할 수 없습니다.&lt;/color&gt;</x:t>
   </x:si>
   <x:si>
-    <x:t>지역 설명(사막)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>지역 설명(습지)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>지역 설명(툰드라)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>이벤트(늪에 빠짐)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>게임 로드 문구</x:t>
-  </x:si>
-  <x:si>
-    <x:t>게임 나가기 문구</x:t>
-  </x:si>
-  <x:si>
-    <x:t>게임 시작 문구</x:t>
-  </x:si>
-  <x:si>
-    <x:t>지역 설명(도시)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>이름(기획자용)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Japanese</x:t>
-  </x:si>
-  <x:si>
-    <x:t>JustoUda</x:t>
+    <x:t>이 구조물은 얼어붙어 있다. 탐사에 오랜 시간이 소요될 것 같다.
+(접근 승인 선택 시 1턴 동안 이동 불가 [선택 시점에 이동 불가])</x:t>
+  </x:si>
+  <x:si>
+    <x:t>생존 프로세스: 배터리 제작</x:t>
+  </x:si>
+  <x:si>
+    <x:t>생존 프로세스: 글리처</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Chinese</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Korean</x:t>
+  </x:si>
+  <x:si>
+    <x:t>이전 게임</x:t>
+  </x:si>
+  <x:si>
+    <x:t>로드 중…</x:t>
+  </x:si>
+  <x:si>
+    <x:t>저장 중…</x:t>
+  </x:si>
+  <x:si>
+    <x:t>게임 저장 중</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Code</x:t>
+  </x:si>
+  <x:si>
+    <x:t>전체 음향</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Justo</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Index</x:t>
+  </x:si>
+  <x:si>
+    <x:t>타이틀 관련</x:t>
+  </x:si>
+  <x:si>
+    <x:t>화면 모드</x:t>
+  </x:si>
+  <x:si>
+    <x:t>전체 화면</x:t>
+  </x:si>
+  <x:si>
+    <x:t>창 모드</x:t>
+  </x:si>
+  <x:si>
+    <x:t>새 게임 시작</x:t>
+  </x:si>
+  <x:si>
+    <x:t>게임 로딩 중</x:t>
+  </x:si>
+  <x:si>
+    <x:t>English</x:t>
+  </x:si>
+  <x:si>
+    <x:t>분석에 따르면 {0}의 보유량이 감소했다고 한다. 소실인가? 혹은 잘못 센 것인가? [{0} 보유량 - 1]</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STR_SELECT_JUSTOUDA_B</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STR_SELECT_JUSTOUDA_KEY</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STR_TILE_JUNGLE_DESC</x:t>
+  </x:si>
+  <x:si>
+    <x:t>교란기 위치의 일정 부분 글리처 무리 정지</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STR_OPTION_SOUND_BGM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STR_NOTE_LOOSE_RESROUCE</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STR_TILE_TUNDRA_DESC</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STR_TITLE_START_GAME</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STR_SELECT_JUSTOUDA_A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STR_OPTION_SOUND_SFX</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STR_NOTE_ACIDENT_ETHER</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STR_TILE_DESERT_DESC</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STR_NEW_NOTICE_ALERT</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STR_OPTION_SOUND_MASTER</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STR_NOTE_DESERT_STORM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STR_NOTE_SEARCH_TUNDRA</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STR_QUEST_TUTORIAL_02</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STR_QUEST_TUTORIAL_06</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STR_QUEST_TUTORIAL_04</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STR_QUEST_TUTORIAL_07</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STR_QUEST_TUTORIAL_03</x:t>
+  </x:si>
+  <x:si>
+    <x:t>주스토</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Uda</x:t>
+  </x:si>
+  <x:si>
+    <x:t>코드</x:t>
+  </x:si>
+  <x:si>
+    <x:t>인덱스</x:t>
+  </x:si>
+  <x:si>
+    <x:t>영어</x:t>
+  </x:si>
+  <x:si>
+    <x:t>효과음</x:t>
+  </x:si>
+  <x:si>
+    <x:t>구분</x:t>
+  </x:si>
+  <x:si>
+    <x:t>화면</x:t>
+  </x:si>
+  <x:si>
+    <x:t>해상도</x:t>
+  </x:si>
+  <x:si>
+    <x:t>설정</x:t>
+  </x:si>
+  <x:si>
+    <x:t>일어</x:t>
+  </x:si>
+  <x:si>
+    <x:t>음향</x:t>
+  </x:si>
+  <x:si>
+    <x:t>배경음</x:t>
+  </x:si>
+  <x:si>
+    <x:t>유다</x:t>
+  </x:si>
+  <x:si>
+    <x:t>중국어</x:t>
+  </x:si>
+  <x:si>
+    <x:t>한국어</x:t>
+  </x:si>
+  <x:si>
+    <x:t>나가기</x:t>
   </x:si>
   <x:si>
     <x:t>&lt;color=red&gt;경고 : 에테르 가스 수집 중 예상치 못한 폭발이 감지되었습니다. 선체 추출 기능이 비활성화되었습니다. 자가 수복 프로토콜을 시작합니다.
 다음 1턴 동안 선체를 이동할 수 없습니다.&lt;/color&gt;</x:t>
   </x:si>
   <x:si>
-    <x:t>구분</x:t>
-  </x:si>
-  <x:si>
-    <x:t>설정</x:t>
-  </x:si>
-  <x:si>
-    <x:t>일어</x:t>
-  </x:si>
-  <x:si>
-    <x:t>효과음</x:t>
-  </x:si>
-  <x:si>
-    <x:t>한국어</x:t>
-  </x:si>
-  <x:si>
-    <x:t>배경음</x:t>
-  </x:si>
-  <x:si>
-    <x:t>화면</x:t>
-  </x:si>
-  <x:si>
-    <x:t>음향</x:t>
-  </x:si>
-  <x:si>
-    <x:t>해상도</x:t>
-  </x:si>
-  <x:si>
-    <x:t>인덱스</x:t>
-  </x:si>
-  <x:si>
-    <x:t>영어</x:t>
-  </x:si>
-  <x:si>
-    <x:t>나가기</x:t>
-  </x:si>
-  <x:si>
-    <x:t>코드</x:t>
-  </x:si>
-  <x:si>
-    <x:t>중국어</x:t>
-  </x:si>
-  <x:si>
-    <x:t>주스토</x:t>
-  </x:si>
-  <x:si>
-    <x:t>유다</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Uda</x:t>
+    <x:t>알림(주변 1타일 글리처 경고)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STR_OPTION_SOUND</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STR_TITLE_EXIT_GAME</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STR_TITLE_SETTING</x:t>
+  </x:si>
+  <x:si>
+    <x:t>탐색기 위치의 일정부분 시야공유</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STR_OPTION_SCREEN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>이벤트(에테르 가스 수집 중 사고)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STR_TITLE_SAVING</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">STR_NOTE_LOOSE_WAY </x:t>
+  </x:si>
+  <x:si>
+    <x:t>STR_DISTRUBTOR_DESC</x:t>
   </x:si>
   <x:si>
     <x:t>STR_TITLE_LOADING</x:t>
   </x:si>
   <x:si>
-    <x:t>STR_OPTION_SCREEN</x:t>
-  </x:si>
-  <x:si>
-    <x:t>STR_TITLE_EXIT_GAME</x:t>
-  </x:si>
-  <x:si>
-    <x:t>STR_TITLE_SAVING</x:t>
-  </x:si>
-  <x:si>
-    <x:t>알림(주변 1타일 글리처 경고)</x:t>
+    <x:t>STR_EXPLORER_DESC</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STR_TILE_CITY_DESC</x:t>
   </x:si>
   <x:si>
     <x:t>STR_TITLE_LOAD_GAME</x:t>
   </x:si>
   <x:si>
-    <x:t>탐색기 위치의 일정부분 시야공유</x:t>
-  </x:si>
-  <x:si>
-    <x:t>이벤트(에테르 가스 수집 중 사고)</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">STR_NOTE_LOOSE_WAY </x:t>
-  </x:si>
-  <x:si>
-    <x:t>STR_OPTION_SOUND</x:t>
-  </x:si>
-  <x:si>
-    <x:t>STR_TILE_CITY_DESC</x:t>
-  </x:si>
-  <x:si>
-    <x:t>STR_TITLE_SETTING</x:t>
-  </x:si>
-  <x:si>
-    <x:t>STR_DISTRUBTOR_DESC</x:t>
-  </x:si>
-  <x:si>
-    <x:t>STR_EXPLORER_DESC</x:t>
-  </x:si>
-  <x:si>
-    <x:t>STR_OPTION_SCREEN_RESOLUTION</x:t>
-  </x:si>
-  <x:si>
-    <x:t>STR_OPTION_SCREEN_FULLSCREEN</x:t>
-  </x:si>
-  <x:si>
-    <x:t>STR_OPTION_SCREEN_SCREENMODE</x:t>
+    <x:t>생산 공장 찾기</x:t>
+  </x:si>
+  <x:si>
+    <x:t>넷 카드 연결하기</x:t>
+  </x:si>
+  <x:si>
+    <x:t>생존 프로세스: 수집</x:t>
+  </x:si>
+  <x:si>
+    <x:t>넷 카드 회수하기</x:t>
+  </x:si>
+  <x:si>
+    <x:t>노트를 열어 생산 공장 조사하기</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STR_QUEST_MAIN_03</x:t>
+  </x:si>
+  <x:si>
+    <x:t>송신 탑 찾기</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STR_QUEST_MAIN_05</x:t>
+  </x:si>
+  <x:si>
+    <x:t>생존 프로세스: 결단</x:t>
+  </x:si>
+  <x:si>
+    <x:t>파괴된 도시 &lt;size=15&gt;포장된 도로 : 선체 이동 거리 + 1&lt;/size&gt;</x:t>
   </x:si>
   <x:si>
     <x:t>&lt;color=red&gt; 경고 : 선체의 방향타 시스템에 오류가 발생하였습니다. 이전에 선택한 경로가 아닌 다른 방향으로 이동하였을 가능성이 있습니다.
 선체 위치를 확인, 조정해 주십시오. &lt;/color&gt;</x:t>
   </x:si>
   <x:si>
-    <x:t>파괴된 도시 &lt;size=15&gt;포장된 도로 : 선체 이동 거리 + 1&lt;/size&gt;</x:t>
-  </x:si>
-  <x:si>
-    <x:t>분석에 따르면 {0}의 보유량이 감소했다고 한다. 소실인가? 혹은 잘못 센 것인가? [{0} 보유량 - 1]</x:t>
-  </x:si>
-  <x:si>
-    <x:t>이 구조물은 얼어붙어 있다. 탐사에 오랜 시간이 소요될 것 같다.
-(접근 승인 선택 시 1턴 동안 이동 불가 [선택 시점에 이동 불가])</x:t>
+    <x:t>STR_OPTION_SCREEN_RESOLUTION</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STR_OPTION_SCREEN_FULLSCREEN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STR_OPTION_SCREEN_SCREENMODE</x:t>
+  </x:si>
+  <x:si>
+    <x:t>툰드라 &lt;size=15&gt;얼어붙은 문 : 구조물 탐사 시 2턴 소모&lt;/size&gt;</x:t>
+  </x:si>
+  <x:si>
+    <x:t>습지 &lt;size=15&gt;풍부한 자원 : 자원 획득 개수 + 1&lt;/size&gt;</x:t>
   </x:si>
   <x:si>
     <x:t>황야 &lt;size=15&gt;부식성 바람 : 턴당 선체 내구도 - 1&lt;/size&gt;</x:t>
   </x:si>
   <x:si>
-    <x:t>툰드라 &lt;size=15&gt;얼어붙은 문 : 구조물 탐사 시 2턴 소모&lt;/size&gt;</x:t>
-  </x:si>
-  <x:si>
-    <x:t>습지 &lt;size=15&gt;풍부한 자원 : 자원 획득 개수 + 1&lt;/size&gt;</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Index</x:t>
-  </x:si>
-  <x:si>
-    <x:t>로드 중…</x:t>
-  </x:si>
-  <x:si>
-    <x:t>타이틀 관련</x:t>
-  </x:si>
-  <x:si>
-    <x:t>화면 모드</x:t>
-  </x:si>
-  <x:si>
-    <x:t>게임 저장 중</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Korean</x:t>
-  </x:si>
-  <x:si>
-    <x:t>저장 중…</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Chinese</x:t>
-  </x:si>
-  <x:si>
-    <x:t>이전 게임</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Code</x:t>
-  </x:si>
-  <x:si>
-    <x:t>전체 음향</x:t>
-  </x:si>
-  <x:si>
-    <x:t>English</x:t>
-  </x:si>
-  <x:si>
-    <x:t>창 모드</x:t>
-  </x:si>
-  <x:si>
-    <x:t>새 게임 시작</x:t>
-  </x:si>
-  <x:si>
-    <x:t>게임 로딩 중</x:t>
-  </x:si>
-  <x:si>
-    <x:t>전체 화면</x:t>
+    <x:t>이벤트(늪에 빠짐)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>지역 설명(사막)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>지역 설명(툰드라)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>게임 로드 문구</x:t>
+  </x:si>
+  <x:si>
+    <x:t>게임 나가기 문구</x:t>
+  </x:si>
+  <x:si>
+    <x:t>지역 설명(습지)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>게임 시작 문구</x:t>
+  </x:si>
+  <x:si>
+    <x:t>지역 설명(도시)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>JustoUda</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Japanese</x:t>
+  </x:si>
+  <x:si>
+    <x:t>이름(기획자용)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STR_OPTION_SCREEN_WINDOWED</x:t>
   </x:si>
   <x:si>
     <x:t>STR_WARNING_NOTICE_ALERT</x:t>
@@ -250,73 +349,34 @@
     <x:t>경고 : 주변 1타일 이내에 글리처가 있습니다.</x:t>
   </x:si>
   <x:si>
-    <x:t>STR_OPTION_SCREEN_WINDOWED</x:t>
-  </x:si>
-  <x:si>
     <x:t>이벤트(툰드라 구조물 탐색)</x:t>
   </x:si>
   <x:si>
     <x:t>새로운 알림이 있습니다.</x:t>
   </x:si>
   <x:si>
+    <x:t>STR_NOTE_SWAMP</x:t>
+  </x:si>
+  <x:si>
+    <x:t>알림(알림 사항 있음)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>이벤트(수풀 속 길잃음)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>이벤트(도둑맞은 자원)</x:t>
+  </x:si>
+  <x:si>
     <x:t>이벤트(사막 모래 폭풍)</x:t>
   </x:si>
   <x:si>
-    <x:t>STR_NOTE_SWAMP</x:t>
-  </x:si>
-  <x:si>
-    <x:t>이벤트(도둑맞은 자원)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>알림(알림 사항 있음)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>이벤트(수풀 속 길잃음)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>STR_OPTION_SOUND_SFX</x:t>
-  </x:si>
-  <x:si>
-    <x:t>STR_TILE_DESERT_DESC</x:t>
-  </x:si>
-  <x:si>
-    <x:t>STR_TILE_JUNGLE_DESC</x:t>
-  </x:si>
-  <x:si>
-    <x:t>STR_NOTE_LOOSE_RESROUCE</x:t>
-  </x:si>
-  <x:si>
-    <x:t>STR_OPTION_SOUND_BGM</x:t>
-  </x:si>
-  <x:si>
-    <x:t>STR_OPTION_SOUND_MASTER</x:t>
-  </x:si>
-  <x:si>
-    <x:t>STR_NOTE_ACIDENT_ETHER</x:t>
-  </x:si>
-  <x:si>
-    <x:t>STR_NOTE_DESERT_STORM</x:t>
-  </x:si>
-  <x:si>
-    <x:t>STR_NEW_NOTICE_ALERT</x:t>
-  </x:si>
-  <x:si>
-    <x:t>STR_NOTE_SEARCH_TUNDRA</x:t>
-  </x:si>
-  <x:si>
-    <x:t>교란기 위치의 일정 부분 글리처 무리 정지</x:t>
-  </x:si>
-  <x:si>
-    <x:t>STR_TILE_TUNDRA_DESC</x:t>
-  </x:si>
-  <x:si>
-    <x:t>STR_TITLE_START_GAME</x:t>
-  </x:si>
-  <x:si>
-    <x:t>STR_SELECT_JUSTOUDA_A</x:t>
-  </x:si>
-  <x:si>
-    <x:t>STR_SELECT_JUSTOUDA_B</x:t>
+    <x:t>STR_QUEST_MAIN_04</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STR_QUEST_MAIN_01</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STR_QUEST_MAIN_02</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -1348,10 +1408,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheetPr codeName="Sheet1"/>
-  <x:dimension ref="A1:H37"/>
+  <x:dimension ref="A1:H46"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <x:selection activeCell="D34" activeCellId="0" sqref="D34:D34"/>
+    <x:sheetView tabSelected="1" topLeftCell="A1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <x:selection activeCell="H44" activeCellId="0" sqref="C2:H44"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="16.399999999999999"/>
@@ -1366,67 +1426,67 @@
   <x:sheetData>
     <x:row r="1" spans="1:8">
       <x:c r="A1" s="14" t="s">
-        <x:v>16</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="B1" s="15" t="s">
-        <x:v>12</x:v>
+        <x:v>104</x:v>
       </x:c>
       <x:c r="C1" s="4" t="s">
-        <x:v>25</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="D1" s="4" t="s">
-        <x:v>28</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="E1" s="4" t="s">
-        <x:v>20</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="F1" s="7" t="s">
-        <x:v>26</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="G1" s="7" t="s">
-        <x:v>18</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="H1" s="7" t="s">
-        <x:v>29</x:v>
+        <x:v>59</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:8">
       <x:c r="A2" s="14"/>
       <x:c r="B2" s="15"/>
       <x:c r="C2" s="5" t="s">
-        <x:v>57</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="D2" s="5" t="s">
-        <x:v>66</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E2" s="5" t="s">
-        <x:v>62</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="F2" s="5" t="s">
-        <x:v>68</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="G2" s="5" t="s">
-        <x:v>13</x:v>
+        <x:v>103</x:v>
       </x:c>
       <x:c r="H2" s="5" t="s">
-        <x:v>64</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:8">
       <x:c r="A3" s="16" t="s">
-        <x:v>59</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="B3" s="8" t="s">
-        <x:v>10</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="C3" s="8">
         <x:v>1001</x:v>
       </x:c>
       <x:c r="D3" s="8" t="s">
-        <x:v>95</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="E3" s="8" t="s">
-        <x:v>70</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="F3" s="8">
         <x:v>-1</x:v>
@@ -1441,16 +1501,16 @@
     <x:row r="4" spans="1:8">
       <x:c r="A4" s="17"/>
       <x:c r="B4" s="8" t="s">
-        <x:v>8</x:v>
+        <x:v>97</x:v>
       </x:c>
       <x:c r="C4" s="8">
         <x:v>1002</x:v>
       </x:c>
       <x:c r="D4" s="8" t="s">
-        <x:v>38</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="E4" s="8" t="s">
-        <x:v>65</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="F4" s="8">
         <x:v>-1</x:v>
@@ -1465,16 +1525,16 @@
     <x:row r="5" spans="1:8">
       <x:c r="A5" s="17"/>
       <x:c r="B5" s="8" t="s">
-        <x:v>9</x:v>
+        <x:v>98</x:v>
       </x:c>
       <x:c r="C5" s="8">
         <x:v>1003</x:v>
       </x:c>
       <x:c r="D5" s="8" t="s">
-        <x:v>35</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="E5" s="8" t="s">
-        <x:v>27</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="F5" s="8">
         <x:v>-1</x:v>
@@ -1489,16 +1549,16 @@
     <x:row r="6" spans="1:8">
       <x:c r="A6" s="17"/>
       <x:c r="B6" s="8" t="s">
-        <x:v>71</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="C6" s="8">
         <x:v>1004</x:v>
       </x:c>
       <x:c r="D6" s="8" t="s">
-        <x:v>33</x:v>
+        <x:v>73</x:v>
       </x:c>
       <x:c r="E6" s="8" t="s">
-        <x:v>58</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="F6" s="8">
         <x:v>-1</x:v>
@@ -1513,16 +1573,16 @@
     <x:row r="7" spans="1:8">
       <x:c r="A7" s="17"/>
       <x:c r="B7" s="8" t="s">
-        <x:v>61</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="C7" s="8">
         <x:v>1005</x:v>
       </x:c>
       <x:c r="D7" s="8" t="s">
-        <x:v>36</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="E7" s="8" t="s">
-        <x:v>63</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="F7" s="8">
         <x:v>-1</x:v>
@@ -1537,16 +1597,16 @@
     <x:row r="8" spans="1:8">
       <x:c r="A8" s="18"/>
       <x:c r="B8" s="8" t="s">
-        <x:v>17</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="C8" s="8">
         <x:v>1006</x:v>
       </x:c>
       <x:c r="D8" s="8" t="s">
-        <x:v>44</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="E8" s="8" t="s">
-        <x:v>17</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="F8" s="8">
         <x:v>-1</x:v>
@@ -1561,16 +1621,16 @@
     <x:row r="9" spans="1:8">
       <x:c r="A9" s="6"/>
       <x:c r="B9" s="9" t="s">
-        <x:v>80</x:v>
+        <x:v>113</x:v>
       </x:c>
       <x:c r="C9" s="9">
         <x:v>2001</x:v>
       </x:c>
       <x:c r="D9" s="9" t="s">
-        <x:v>86</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="E9" s="9" t="s">
-        <x:v>52</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="F9" s="9">
         <x:v>-1</x:v>
@@ -1585,16 +1645,16 @@
     <x:row r="10" spans="1:8">
       <x:c r="A10" s="6"/>
       <x:c r="B10" s="9" t="s">
-        <x:v>78</x:v>
+        <x:v>114</x:v>
       </x:c>
       <x:c r="C10" s="9">
         <x:v>2002</x:v>
       </x:c>
       <x:c r="D10" s="9" t="s">
-        <x:v>90</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="E10" s="9" t="s">
-        <x:v>2</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="F10" s="9">
         <x:v>-1</x:v>
@@ -1609,16 +1669,16 @@
     <x:row r="11" spans="1:8" ht="32.75">
       <x:c r="A11" s="6"/>
       <x:c r="B11" s="9" t="s">
-        <x:v>76</x:v>
+        <x:v>108</x:v>
       </x:c>
       <x:c r="C11" s="9">
         <x:v>2003</x:v>
       </x:c>
       <x:c r="D11" s="9" t="s">
-        <x:v>92</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="E11" s="10" t="s">
-        <x:v>53</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="F11" s="9">
         <x:v>-1</x:v>
@@ -1633,16 +1693,16 @@
     <x:row r="12" spans="1:8" ht="49.149999999999999">
       <x:c r="A12" s="6"/>
       <x:c r="B12" s="9" t="s">
-        <x:v>40</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="C12" s="9">
         <x:v>2004</x:v>
       </x:c>
       <x:c r="D12" s="9" t="s">
-        <x:v>89</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="E12" s="10" t="s">
-        <x:v>15</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="F12" s="9">
         <x:v>-1</x:v>
@@ -1657,16 +1717,16 @@
     <x:row r="13" spans="1:8" ht="49.149999999999999">
       <x:c r="A13" s="6"/>
       <x:c r="B13" s="9" t="s">
-        <x:v>82</x:v>
+        <x:v>112</x:v>
       </x:c>
       <x:c r="C13" s="9">
         <x:v>2005</x:v>
       </x:c>
       <x:c r="D13" s="9" t="s">
-        <x:v>41</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="E13" s="10" t="s">
-        <x:v>50</x:v>
+        <x:v>87</x:v>
       </x:c>
       <x:c r="F13" s="9">
         <x:v>-1</x:v>
@@ -1681,16 +1741,16 @@
     <x:row r="14" spans="1:8" ht="32.75">
       <x:c r="A14" s="6"/>
       <x:c r="B14" s="9" t="s">
-        <x:v>7</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="C14" s="9">
         <x:v>2006</x:v>
       </x:c>
       <x:c r="D14" s="9" t="s">
-        <x:v>79</x:v>
+        <x:v>110</x:v>
       </x:c>
       <x:c r="E14" s="10" t="s">
-        <x:v>3</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="F14" s="9">
         <x:v>-1</x:v>
@@ -1705,16 +1765,16 @@
     <x:row r="15" spans="1:8">
       <x:c r="A15" s="6"/>
       <x:c r="B15" s="11" t="s">
-        <x:v>11</x:v>
+        <x:v>101</x:v>
       </x:c>
       <x:c r="C15" s="11">
         <x:v>3001</x:v>
       </x:c>
       <x:c r="D15" s="11" t="s">
-        <x:v>43</x:v>
+        <x:v>75</x:v>
       </x:c>
       <x:c r="E15" s="12" t="s">
-        <x:v>51</x:v>
+        <x:v>86</x:v>
       </x:c>
       <x:c r="F15" s="11">
         <x:v>-1</x:v>
@@ -1729,16 +1789,16 @@
     <x:row r="16" spans="1:8">
       <x:c r="A16" s="6"/>
       <x:c r="B16" s="11" t="s">
-        <x:v>5</x:v>
+        <x:v>99</x:v>
       </x:c>
       <x:c r="C16" s="11">
         <x:v>3002</x:v>
       </x:c>
       <x:c r="D16" s="11" t="s">
-        <x:v>85</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="E16" s="12" t="s">
-        <x:v>56</x:v>
+        <x:v>92</x:v>
       </x:c>
       <x:c r="F16" s="11">
         <x:v>-1</x:v>
@@ -1753,16 +1813,16 @@
     <x:row r="17" spans="1:8">
       <x:c r="A17" s="6"/>
       <x:c r="B17" s="11" t="s">
-        <x:v>4</x:v>
+        <x:v>95</x:v>
       </x:c>
       <x:c r="C17" s="11">
         <x:v>3003</x:v>
       </x:c>
       <x:c r="D17" s="11" t="s">
-        <x:v>84</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="E17" s="12" t="s">
-        <x:v>54</x:v>
+        <x:v>93</x:v>
       </x:c>
       <x:c r="F17" s="11">
         <x:v>-1</x:v>
@@ -1777,16 +1837,16 @@
     <x:row r="18" spans="1:8">
       <x:c r="A18" s="6"/>
       <x:c r="B18" s="11" t="s">
-        <x:v>6</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="C18" s="11">
         <x:v>3004</x:v>
       </x:c>
       <x:c r="D18" s="11" t="s">
-        <x:v>94</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="E18" s="12" t="s">
-        <x:v>55</x:v>
+        <x:v>91</x:v>
       </x:c>
       <x:c r="F18" s="11">
         <x:v>-1</x:v>
@@ -1801,16 +1861,16 @@
     <x:row r="19" spans="1:8">
       <x:c r="A19" s="6"/>
       <x:c r="B19" s="13" t="s">
-        <x:v>81</x:v>
+        <x:v>111</x:v>
       </x:c>
       <x:c r="C19" s="13">
         <x:v>4001</x:v>
       </x:c>
       <x:c r="D19" s="13" t="s">
-        <x:v>91</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="E19" s="13" t="s">
-        <x:v>77</x:v>
+        <x:v>109</x:v>
       </x:c>
       <x:c r="F19" s="13">
         <x:v>-1</x:v>
@@ -1825,16 +1885,16 @@
     <x:row r="20" spans="1:8">
       <x:c r="A20" s="6"/>
       <x:c r="B20" s="13" t="s">
-        <x:v>37</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="C20" s="13">
         <x:v>4002</x:v>
       </x:c>
       <x:c r="D20" s="13" t="s">
-        <x:v>73</x:v>
+        <x:v>106</x:v>
       </x:c>
       <x:c r="E20" s="13" t="s">
-        <x:v>74</x:v>
+        <x:v>107</x:v>
       </x:c>
       <x:c r="F20" s="13">
         <x:v>-1</x:v>
@@ -1853,10 +1913,10 @@
         <x:v>5001</x:v>
       </x:c>
       <x:c r="D21" s="6" t="s">
-        <x:v>42</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="E21" s="6" t="s">
-        <x:v>23</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="F21" s="6">
         <x:v>-1</x:v>
@@ -1875,10 +1935,10 @@
         <x:v>5002</x:v>
       </x:c>
       <x:c r="D22" s="6" t="s">
-        <x:v>88</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="E22" s="6" t="s">
-        <x:v>67</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="F22" s="6">
         <x:v>-1</x:v>
@@ -1897,10 +1957,10 @@
         <x:v>5003</x:v>
       </x:c>
       <x:c r="D23" s="6" t="s">
-        <x:v>87</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="E23" s="6" t="s">
-        <x:v>21</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="F23" s="6">
         <x:v>-1</x:v>
@@ -1919,10 +1979,10 @@
         <x:v>5004</x:v>
       </x:c>
       <x:c r="D24" s="6" t="s">
-        <x:v>83</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="E24" s="6" t="s">
-        <x:v>19</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="F24" s="6">
         <x:v>-1</x:v>
@@ -1941,10 +2001,10 @@
         <x:v>5005</x:v>
       </x:c>
       <x:c r="D25" s="6" t="s">
-        <x:v>34</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="E25" s="6" t="s">
-        <x:v>22</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="F25" s="6">
         <x:v>-1</x:v>
@@ -1963,10 +2023,10 @@
         <x:v>5006</x:v>
       </x:c>
       <x:c r="D26" s="6" t="s">
-        <x:v>49</x:v>
+        <x:v>90</x:v>
       </x:c>
       <x:c r="E26" s="6" t="s">
-        <x:v>60</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="F26" s="6">
         <x:v>-1</x:v>
@@ -1985,10 +2045,10 @@
         <x:v>5007</x:v>
       </x:c>
       <x:c r="D27" s="6" t="s">
-        <x:v>48</x:v>
+        <x:v>89</x:v>
       </x:c>
       <x:c r="E27" s="6" t="s">
-        <x:v>72</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="F27" s="6">
         <x:v>-1</x:v>
@@ -2007,10 +2067,10 @@
         <x:v>5008</x:v>
       </x:c>
       <x:c r="D28" s="6" t="s">
-        <x:v>75</x:v>
+        <x:v>105</x:v>
       </x:c>
       <x:c r="E28" s="6" t="s">
-        <x:v>69</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="F28" s="6">
         <x:v>-1</x:v>
@@ -2029,10 +2089,10 @@
         <x:v>5009</x:v>
       </x:c>
       <x:c r="D29" s="6" t="s">
-        <x:v>47</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="E29" s="6" t="s">
-        <x:v>24</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="F29" s="6">
         <x:v>-1</x:v>
@@ -2051,10 +2111,10 @@
         <x:v>6001</x:v>
       </x:c>
       <x:c r="D30" s="6" t="s">
-        <x:v>45</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="E30" s="6" t="s">
-        <x:v>93</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="F30" s="6">
         <x:v>-1</x:v>
@@ -2073,10 +2133,10 @@
         <x:v>6002</x:v>
       </x:c>
       <x:c r="D31" s="6" t="s">
-        <x:v>46</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="E31" s="6" t="s">
-        <x:v>39</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="F31" s="6">
         <x:v>-1</x:v>
@@ -2095,19 +2155,19 @@
         <x:v>7001</x:v>
       </x:c>
       <x:c r="D32" s="6" t="s">
-        <x:v>0</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="E32" s="6" t="s">
-        <x:v>14</x:v>
+        <x:v>102</x:v>
       </x:c>
       <x:c r="F32" s="6" t="s">
-        <x:v>14</x:v>
+        <x:v>102</x:v>
       </x:c>
       <x:c r="G32" s="6" t="s">
-        <x:v>14</x:v>
+        <x:v>102</x:v>
       </x:c>
       <x:c r="H32" s="6" t="s">
-        <x:v>14</x:v>
+        <x:v>102</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:8">
@@ -2117,13 +2177,13 @@
         <x:v>7002</x:v>
       </x:c>
       <x:c r="D33" s="6" t="s">
-        <x:v>96</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="E33" s="6" t="s">
-        <x:v>30</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="F33" s="6" t="s">
-        <x:v>1</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="G33" s="6">
         <x:v>-1</x:v>
@@ -2139,13 +2199,13 @@
         <x:v>7003</x:v>
       </x:c>
       <x:c r="D34" s="6" t="s">
-        <x:v>97</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="E34" s="6" t="s">
-        <x:v>31</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="F34" s="6" t="s">
-        <x:v>32</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="G34" s="6">
         <x:v>-1</x:v>
@@ -2157,9 +2217,15 @@
     <x:row r="35" spans="1:8">
       <x:c r="A35" s="6"/>
       <x:c r="B35" s="6"/>
-      <x:c r="C35" s="6"/>
-      <x:c r="D35" s="6"/>
-      <x:c r="E35" s="6"/>
+      <x:c r="C35" s="6">
+        <x:v>8001</x:v>
+      </x:c>
+      <x:c r="D35" s="6" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="E35" s="6" t="s">
+        <x:v>4</x:v>
+      </x:c>
       <x:c r="F35" s="6">
         <x:v>-1</x:v>
       </x:c>
@@ -2173,9 +2239,15 @@
     <x:row r="36" spans="1:8">
       <x:c r="A36" s="6"/>
       <x:c r="B36" s="6"/>
-      <x:c r="C36" s="6"/>
-      <x:c r="D36" s="6"/>
-      <x:c r="E36" s="6"/>
+      <x:c r="C36" s="6">
+        <x:v>8002</x:v>
+      </x:c>
+      <x:c r="D36" s="6" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="E36" s="6" t="s">
+        <x:v>85</x:v>
+      </x:c>
       <x:c r="F36" s="6">
         <x:v>-1</x:v>
       </x:c>
@@ -2189,9 +2261,15 @@
     <x:row r="37" spans="1:8">
       <x:c r="A37" s="6"/>
       <x:c r="B37" s="6"/>
-      <x:c r="C37" s="6"/>
-      <x:c r="D37" s="6"/>
-      <x:c r="E37" s="6"/>
+      <x:c r="C37" s="6">
+        <x:v>8003</x:v>
+      </x:c>
+      <x:c r="D37" s="6" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="E37" s="6" t="s">
+        <x:v>5</x:v>
+      </x:c>
       <x:c r="F37" s="6">
         <x:v>-1</x:v>
       </x:c>
@@ -2199,6 +2277,178 @@
         <x:v>-1</x:v>
       </x:c>
       <x:c r="H37" s="6">
+        <x:v>-1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="38" spans="3:8">
+      <x:c r="C38" s="6">
+        <x:v>8004</x:v>
+      </x:c>
+      <x:c r="D38" s="6" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="E38" s="6" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="F38" s="6">
+        <x:v>-1</x:v>
+      </x:c>
+      <x:c r="G38" s="6">
+        <x:v>-1</x:v>
+      </x:c>
+      <x:c r="H38" s="6">
+        <x:v>-1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="39" spans="3:8">
+      <x:c r="C39" s="6">
+        <x:v>8005</x:v>
+      </x:c>
+      <x:c r="D39" s="6" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="E39" s="6" t="s">
+        <x:v>79</x:v>
+      </x:c>
+      <x:c r="F39" s="6">
+        <x:v>-1</x:v>
+      </x:c>
+      <x:c r="G39" s="6">
+        <x:v>-1</x:v>
+      </x:c>
+      <x:c r="H39" s="6">
+        <x:v>-1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="40" spans="3:8">
+      <x:c r="C40" s="6">
+        <x:v>8006</x:v>
+      </x:c>
+      <x:c r="D40" s="6" t="s">
+        <x:v>116</x:v>
+      </x:c>
+      <x:c r="E40" s="6" t="s">
+        <x:v>77</x:v>
+      </x:c>
+      <x:c r="F40" s="6">
+        <x:v>-1</x:v>
+      </x:c>
+      <x:c r="G40" s="6">
+        <x:v>-1</x:v>
+      </x:c>
+      <x:c r="H40" s="6">
+        <x:v>-1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="41" spans="3:8">
+      <x:c r="C41" s="6">
+        <x:v>8007</x:v>
+      </x:c>
+      <x:c r="D41" s="6" t="s">
+        <x:v>117</x:v>
+      </x:c>
+      <x:c r="E41" s="6" t="s">
+        <x:v>81</x:v>
+      </x:c>
+      <x:c r="F41" s="6">
+        <x:v>-1</x:v>
+      </x:c>
+      <x:c r="G41" s="6">
+        <x:v>-1</x:v>
+      </x:c>
+      <x:c r="H41" s="6">
+        <x:v>-1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="42" spans="3:8">
+      <x:c r="C42" s="6">
+        <x:v>8008</x:v>
+      </x:c>
+      <x:c r="D42" s="6" t="s">
+        <x:v>82</x:v>
+      </x:c>
+      <x:c r="E42" s="6" t="s">
+        <x:v>80</x:v>
+      </x:c>
+      <x:c r="F42" s="6">
+        <x:v>-1</x:v>
+      </x:c>
+      <x:c r="G42" s="6">
+        <x:v>-1</x:v>
+      </x:c>
+      <x:c r="H42" s="6">
+        <x:v>-1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="43" spans="3:8">
+      <x:c r="C43" s="6">
+        <x:v>8009</x:v>
+      </x:c>
+      <x:c r="D43" s="6" t="s">
+        <x:v>115</x:v>
+      </x:c>
+      <x:c r="E43" s="6" t="s">
+        <x:v>83</x:v>
+      </x:c>
+      <x:c r="F43" s="6">
+        <x:v>-1</x:v>
+      </x:c>
+      <x:c r="G43" s="6">
+        <x:v>-1</x:v>
+      </x:c>
+      <x:c r="H43" s="6">
+        <x:v>-1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="44" spans="3:8">
+      <x:c r="C44" s="6">
+        <x:v>8010</x:v>
+      </x:c>
+      <x:c r="D44" s="6" t="s">
+        <x:v>84</x:v>
+      </x:c>
+      <x:c r="E44" s="6" t="s">
+        <x:v>78</x:v>
+      </x:c>
+      <x:c r="F44" s="6">
+        <x:v>-1</x:v>
+      </x:c>
+      <x:c r="G44" s="6">
+        <x:v>-1</x:v>
+      </x:c>
+      <x:c r="H44" s="6">
+        <x:v>-1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="45" spans="3:8">
+      <x:c r="C45" s="6">
+        <x:v>8011</x:v>
+      </x:c>
+      <x:c r="D45" s="6"/>
+      <x:c r="E45" s="6"/>
+      <x:c r="F45" s="6">
+        <x:v>-1</x:v>
+      </x:c>
+      <x:c r="G45" s="6">
+        <x:v>-1</x:v>
+      </x:c>
+      <x:c r="H45" s="6">
+        <x:v>-1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="46" spans="3:8">
+      <x:c r="C46" s="6">
+        <x:v>8012</x:v>
+      </x:c>
+      <x:c r="D46" s="6"/>
+      <x:c r="E46" s="6"/>
+      <x:c r="F46" s="6">
+        <x:v>-1</x:v>
+      </x:c>
+      <x:c r="G46" s="6">
+        <x:v>-1</x:v>
+      </x:c>
+      <x:c r="H46" s="6">
         <x:v>-1</x:v>
       </x:c>
     </x:row>

</xml_diff>

<commit_message>
[Mod]: Disturb -> Disruptor / Findor -> Explorer 명칭 통일
</commit_message>
<xml_diff>
--- a/Assets/10.Data/StringTable.xlsx
+++ b/Assets/10.Data/StringTable.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <x:bookViews>
-    <x:workbookView xWindow="0" yWindow="0" windowWidth="21690" windowHeight="11655"/>
+    <x:workbookView xWindow="0" yWindow="0" windowWidth="28545" windowHeight="12210"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="Sheet1" sheetId="1" r:id="rId4"/>
@@ -21,362 +21,362 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="118">
   <x:si>
-    <x:t>생존 프로세스: 도망</x:t>
-  </x:si>
-  <x:si>
-    <x:t>&lt;color=red&gt; 경고 : 강력한 모래 폭풍이 감지되었습니다. 강제 안전 조율 시스템을 가동합니다. 다음 1턴동안 선체를 이동할 수 없습니다. &lt;/color&gt;</x:t>
+    <x:t>&lt;color=red&gt;경고 : 에테르 가스 수집 중 예상치 못한 폭발이 감지되었습니다. 선체 추출 기능이 비활성화되었습니다. 자가 수복 프로토콜을 시작합니다.
+다음 1턴 동안 선체를 이동할 수 없습니다.&lt;/color&gt;</x:t>
+  </x:si>
+  <x:si>
+    <x:t>분석에 따르면 {0}의 보유량이 감소했다고 한다. 소실인가? 혹은 잘못 센 것인가? [{0} 보유량 - 1]</x:t>
   </x:si>
   <x:si>
     <x:t>&lt;color=red&gt; 경고 : 선체가 정글의 거대한 늪에 빠졌습니다. 자가 수복 프로토콜을 시작합니다.
 다음 1턴 동안 선체를 이동할 수 없습니다.&lt;/color&gt;</x:t>
   </x:si>
   <x:si>
+    <x:t>&lt;color=red&gt; 경고 : 강력한 모래 폭풍이 감지되었습니다. 강제 안전 조율 시스템을 가동합니다. 다음 1턴동안 선체를 이동할 수 없습니다. &lt;/color&gt;</x:t>
+  </x:si>
+  <x:si>
+    <x:t>&lt;color=red&gt; 경고 : 선체의 방향타 시스템에 오류가 발생하였습니다. 이전에 선택한 경로가 아닌 다른 방향으로 이동하였을 가능성이 있습니다.
+선체 위치를 확인, 조정해 주십시오. &lt;/color&gt;</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STR_OPTION_SCREEN_SCREENMODE</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STR_OPTION_SCREEN_FULLSCREEN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STR_OPTION_SCREEN_RESOLUTION</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STR_TILE_CITY_DESC</x:t>
+  </x:si>
+  <x:si>
+    <x:t>이벤트(에테르 가스 수집 중 사고)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STR_QUEST_MAIN_05</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STR_OPTION_SCREEN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STR_TITLE_LOAD_GAME</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STR_TITLE_LOADING</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STR_QUEST_MAIN_02</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STR_TITLE_SAVING</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STR_QUEST_MAIN_03</x:t>
+  </x:si>
+  <x:si>
+    <x:t>탐색기 위치의 일정부분 시야공유</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">STR_NOTE_LOOSE_WAY </x:t>
+  </x:si>
+  <x:si>
+    <x:t>노트를 열어 생산 공장 조사하기</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STR_QUEST_MAIN_01</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STR_EXPLORER_DESC</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STR_QUEST_MAIN_04</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STR_OPTION_SOUND</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STR_TITLE_EXIT_GAME</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STR_TITLE_SETTING</x:t>
+  </x:si>
+  <x:si>
+    <x:t>알림(주변 1타일 글리처 경고)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STR_SELECT_JUSTOUDA_B</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STR_TILE_JUNGLE_DESC</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STR_TILE_TUNDRA_DESC</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STR_TITLE_START_GAME</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STR_TILE_DESERT_DESC</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STR_SELECT_JUSTOUDA_KEY</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STR_SELECT_JUSTOUDA_A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STR_NOTE_ACIDENT_ETHER</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STR_NEW_NOTICE_ALERT</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STR_NOTE_DESERT_STORM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STR_QUEST_TUTORIAL_06</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STR_QUEST_TUTORIAL_02</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STR_NOTE_SEARCH_TUNDRA</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STR_QUEST_TUTORIAL_03</x:t>
+  </x:si>
+  <x:si>
+    <x:t>교란기 위치의 일정 부분 글리처 무리 정지</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STR_NOTE_LOOSE_RESROUCE</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STR_QUEST_TUTORIAL_07</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STR_OPTION_SOUND_BGM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STR_OPTION_SOUND_SFX</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STR_QUEST_TUTORIAL_04</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STR_OPTION_SOUND_MASTER</x:t>
+  </x:si>
+  <x:si>
+    <x:t>음향</x:t>
+  </x:si>
+  <x:si>
+    <x:t>화면</x:t>
+  </x:si>
+  <x:si>
+    <x:t>구분</x:t>
+  </x:si>
+  <x:si>
+    <x:t>배경음</x:t>
+  </x:si>
+  <x:si>
+    <x:t>중국어</x:t>
+  </x:si>
+  <x:si>
+    <x:t>한국어</x:t>
+  </x:si>
+  <x:si>
+    <x:t>유다</x:t>
+  </x:si>
+  <x:si>
+    <x:t>코드</x:t>
+  </x:si>
+  <x:si>
+    <x:t>주스토</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Uda</x:t>
+  </x:si>
+  <x:si>
+    <x:t>해상도</x:t>
+  </x:si>
+  <x:si>
+    <x:t>인덱스</x:t>
+  </x:si>
+  <x:si>
+    <x:t>설정</x:t>
+  </x:si>
+  <x:si>
+    <x:t>일어</x:t>
+  </x:si>
+  <x:si>
+    <x:t>효과음</x:t>
+  </x:si>
+  <x:si>
+    <x:t>영어</x:t>
+  </x:si>
+  <x:si>
+    <x:t>나가기</x:t>
+  </x:si>
+  <x:si>
+    <x:t>생존 프로세스: 도망</x:t>
+  </x:si>
+  <x:si>
+    <x:t>생존 프로세스: 결단</x:t>
+  </x:si>
+  <x:si>
+    <x:t>생존 프로세스: 수집</x:t>
+  </x:si>
+  <x:si>
+    <x:t>넷 카드 회수하기</x:t>
+  </x:si>
+  <x:si>
+    <x:t>넷 카드 연결하기</x:t>
+  </x:si>
+  <x:si>
+    <x:t>생산 공장 찾기</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Japanese</x:t>
+  </x:si>
+  <x:si>
+    <x:t>이벤트(늪에 빠짐)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>지역 설명(사막)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>지역 설명(도시)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>JustoUda</x:t>
+  </x:si>
+  <x:si>
+    <x:t>게임 로드 문구</x:t>
+  </x:si>
+  <x:si>
+    <x:t>게임 나가기 문구</x:t>
+  </x:si>
+  <x:si>
+    <x:t>게임 시작 문구</x:t>
+  </x:si>
+  <x:si>
+    <x:t>이름(기획자용)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>지역 설명(습지)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>지역 설명(툰드라)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>파괴된 도시 &lt;size=15&gt;포장된 도로 : 선체 이동 거리 + 1&lt;/size&gt;</x:t>
+  </x:si>
+  <x:si>
+    <x:t>황야 &lt;size=15&gt;부식성 바람 : 턴당 선체 내구도 - 1&lt;/size&gt;</x:t>
+  </x:si>
+  <x:si>
+    <x:t>습지 &lt;size=15&gt;풍부한 자원 : 자원 획득 개수 + 1&lt;/size&gt;</x:t>
+  </x:si>
+  <x:si>
+    <x:t>툰드라 &lt;size=15&gt;얼어붙은 문 : 구조물 탐사 시 2턴 소모&lt;/size&gt;</x:t>
+  </x:si>
+  <x:si>
     <x:t>이 구조물은 얼어붙어 있다. 탐사에 오랜 시간이 소요될 것 같다.
 (접근 승인 선택 시 1턴 동안 이동 불가 [선택 시점에 이동 불가])</x:t>
   </x:si>
   <x:si>
+    <x:t>English</x:t>
+  </x:si>
+  <x:si>
+    <x:t>송신 탑 찾기</x:t>
+  </x:si>
+  <x:si>
+    <x:t>전체 음향</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Code</x:t>
+  </x:si>
+  <x:si>
+    <x:t>새 게임 시작</x:t>
+  </x:si>
+  <x:si>
+    <x:t>전체 화면</x:t>
+  </x:si>
+  <x:si>
+    <x:t>게임 저장 중</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Index</x:t>
+  </x:si>
+  <x:si>
+    <x:t>화면 모드</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Justo</x:t>
+  </x:si>
+  <x:si>
+    <x:t>타이틀 관련</x:t>
+  </x:si>
+  <x:si>
+    <x:t>게임 로딩 중</x:t>
+  </x:si>
+  <x:si>
+    <x:t>창 모드</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Korean</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Chinese</x:t>
+  </x:si>
+  <x:si>
+    <x:t>이전 게임</x:t>
+  </x:si>
+  <x:si>
+    <x:t>로드 중…</x:t>
+  </x:si>
+  <x:si>
+    <x:t>저장 중…</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STR_DISRUPTOR_DESC</x:t>
+  </x:si>
+  <x:si>
     <x:t>생존 프로세스: 배터리 제작</x:t>
   </x:si>
   <x:si>
+    <x:t>새로운 알림이 있습니다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>이벤트(도둑맞은 자원)</x:t>
+  </x:si>
+  <x:si>
     <x:t>생존 프로세스: 글리처</x:t>
   </x:si>
   <x:si>
-    <x:t>Chinese</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Korean</x:t>
-  </x:si>
-  <x:si>
-    <x:t>이전 게임</x:t>
-  </x:si>
-  <x:si>
-    <x:t>로드 중…</x:t>
-  </x:si>
-  <x:si>
-    <x:t>저장 중…</x:t>
-  </x:si>
-  <x:si>
-    <x:t>게임 저장 중</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Code</x:t>
-  </x:si>
-  <x:si>
-    <x:t>전체 음향</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Justo</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Index</x:t>
-  </x:si>
-  <x:si>
-    <x:t>타이틀 관련</x:t>
-  </x:si>
-  <x:si>
-    <x:t>화면 모드</x:t>
-  </x:si>
-  <x:si>
-    <x:t>전체 화면</x:t>
-  </x:si>
-  <x:si>
-    <x:t>창 모드</x:t>
-  </x:si>
-  <x:si>
-    <x:t>새 게임 시작</x:t>
-  </x:si>
-  <x:si>
-    <x:t>게임 로딩 중</x:t>
-  </x:si>
-  <x:si>
-    <x:t>English</x:t>
-  </x:si>
-  <x:si>
-    <x:t>분석에 따르면 {0}의 보유량이 감소했다고 한다. 소실인가? 혹은 잘못 센 것인가? [{0} 보유량 - 1]</x:t>
-  </x:si>
-  <x:si>
-    <x:t>STR_SELECT_JUSTOUDA_B</x:t>
-  </x:si>
-  <x:si>
-    <x:t>STR_SELECT_JUSTOUDA_KEY</x:t>
-  </x:si>
-  <x:si>
-    <x:t>STR_TILE_JUNGLE_DESC</x:t>
-  </x:si>
-  <x:si>
-    <x:t>교란기 위치의 일정 부분 글리처 무리 정지</x:t>
-  </x:si>
-  <x:si>
-    <x:t>STR_OPTION_SOUND_BGM</x:t>
-  </x:si>
-  <x:si>
-    <x:t>STR_NOTE_LOOSE_RESROUCE</x:t>
-  </x:si>
-  <x:si>
-    <x:t>STR_TILE_TUNDRA_DESC</x:t>
-  </x:si>
-  <x:si>
-    <x:t>STR_TITLE_START_GAME</x:t>
-  </x:si>
-  <x:si>
-    <x:t>STR_SELECT_JUSTOUDA_A</x:t>
-  </x:si>
-  <x:si>
-    <x:t>STR_OPTION_SOUND_SFX</x:t>
-  </x:si>
-  <x:si>
-    <x:t>STR_NOTE_ACIDENT_ETHER</x:t>
-  </x:si>
-  <x:si>
-    <x:t>STR_TILE_DESERT_DESC</x:t>
-  </x:si>
-  <x:si>
-    <x:t>STR_NEW_NOTICE_ALERT</x:t>
-  </x:si>
-  <x:si>
-    <x:t>STR_OPTION_SOUND_MASTER</x:t>
-  </x:si>
-  <x:si>
-    <x:t>STR_NOTE_DESERT_STORM</x:t>
-  </x:si>
-  <x:si>
-    <x:t>STR_NOTE_SEARCH_TUNDRA</x:t>
-  </x:si>
-  <x:si>
-    <x:t>STR_QUEST_TUTORIAL_02</x:t>
-  </x:si>
-  <x:si>
-    <x:t>STR_QUEST_TUTORIAL_06</x:t>
-  </x:si>
-  <x:si>
-    <x:t>STR_QUEST_TUTORIAL_04</x:t>
-  </x:si>
-  <x:si>
-    <x:t>STR_QUEST_TUTORIAL_07</x:t>
-  </x:si>
-  <x:si>
-    <x:t>STR_QUEST_TUTORIAL_03</x:t>
-  </x:si>
-  <x:si>
-    <x:t>주스토</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Uda</x:t>
-  </x:si>
-  <x:si>
-    <x:t>코드</x:t>
-  </x:si>
-  <x:si>
-    <x:t>인덱스</x:t>
-  </x:si>
-  <x:si>
-    <x:t>영어</x:t>
-  </x:si>
-  <x:si>
-    <x:t>효과음</x:t>
-  </x:si>
-  <x:si>
-    <x:t>구분</x:t>
-  </x:si>
-  <x:si>
-    <x:t>화면</x:t>
-  </x:si>
-  <x:si>
-    <x:t>해상도</x:t>
-  </x:si>
-  <x:si>
-    <x:t>설정</x:t>
-  </x:si>
-  <x:si>
-    <x:t>일어</x:t>
-  </x:si>
-  <x:si>
-    <x:t>음향</x:t>
-  </x:si>
-  <x:si>
-    <x:t>배경음</x:t>
-  </x:si>
-  <x:si>
-    <x:t>유다</x:t>
-  </x:si>
-  <x:si>
-    <x:t>중국어</x:t>
-  </x:si>
-  <x:si>
-    <x:t>한국어</x:t>
-  </x:si>
-  <x:si>
-    <x:t>나가기</x:t>
-  </x:si>
-  <x:si>
-    <x:t>&lt;color=red&gt;경고 : 에테르 가스 수집 중 예상치 못한 폭발이 감지되었습니다. 선체 추출 기능이 비활성화되었습니다. 자가 수복 프로토콜을 시작합니다.
-다음 1턴 동안 선체를 이동할 수 없습니다.&lt;/color&gt;</x:t>
-  </x:si>
-  <x:si>
-    <x:t>알림(주변 1타일 글리처 경고)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>STR_OPTION_SOUND</x:t>
-  </x:si>
-  <x:si>
-    <x:t>STR_TITLE_EXIT_GAME</x:t>
-  </x:si>
-  <x:si>
-    <x:t>STR_TITLE_SETTING</x:t>
-  </x:si>
-  <x:si>
-    <x:t>탐색기 위치의 일정부분 시야공유</x:t>
-  </x:si>
-  <x:si>
-    <x:t>STR_OPTION_SCREEN</x:t>
-  </x:si>
-  <x:si>
-    <x:t>이벤트(에테르 가스 수집 중 사고)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>STR_TITLE_SAVING</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">STR_NOTE_LOOSE_WAY </x:t>
-  </x:si>
-  <x:si>
-    <x:t>STR_DISTRUBTOR_DESC</x:t>
-  </x:si>
-  <x:si>
-    <x:t>STR_TITLE_LOADING</x:t>
-  </x:si>
-  <x:si>
-    <x:t>STR_EXPLORER_DESC</x:t>
-  </x:si>
-  <x:si>
-    <x:t>STR_TILE_CITY_DESC</x:t>
-  </x:si>
-  <x:si>
-    <x:t>STR_TITLE_LOAD_GAME</x:t>
-  </x:si>
-  <x:si>
-    <x:t>생산 공장 찾기</x:t>
-  </x:si>
-  <x:si>
-    <x:t>넷 카드 연결하기</x:t>
-  </x:si>
-  <x:si>
-    <x:t>생존 프로세스: 수집</x:t>
-  </x:si>
-  <x:si>
-    <x:t>넷 카드 회수하기</x:t>
-  </x:si>
-  <x:si>
-    <x:t>노트를 열어 생산 공장 조사하기</x:t>
-  </x:si>
-  <x:si>
-    <x:t>STR_QUEST_MAIN_03</x:t>
-  </x:si>
-  <x:si>
-    <x:t>송신 탑 찾기</x:t>
-  </x:si>
-  <x:si>
-    <x:t>STR_QUEST_MAIN_05</x:t>
-  </x:si>
-  <x:si>
-    <x:t>생존 프로세스: 결단</x:t>
-  </x:si>
-  <x:si>
-    <x:t>파괴된 도시 &lt;size=15&gt;포장된 도로 : 선체 이동 거리 + 1&lt;/size&gt;</x:t>
-  </x:si>
-  <x:si>
-    <x:t>&lt;color=red&gt; 경고 : 선체의 방향타 시스템에 오류가 발생하였습니다. 이전에 선택한 경로가 아닌 다른 방향으로 이동하였을 가능성이 있습니다.
-선체 위치를 확인, 조정해 주십시오. &lt;/color&gt;</x:t>
-  </x:si>
-  <x:si>
-    <x:t>STR_OPTION_SCREEN_RESOLUTION</x:t>
-  </x:si>
-  <x:si>
-    <x:t>STR_OPTION_SCREEN_FULLSCREEN</x:t>
-  </x:si>
-  <x:si>
-    <x:t>STR_OPTION_SCREEN_SCREENMODE</x:t>
-  </x:si>
-  <x:si>
-    <x:t>툰드라 &lt;size=15&gt;얼어붙은 문 : 구조물 탐사 시 2턴 소모&lt;/size&gt;</x:t>
-  </x:si>
-  <x:si>
-    <x:t>습지 &lt;size=15&gt;풍부한 자원 : 자원 획득 개수 + 1&lt;/size&gt;</x:t>
-  </x:si>
-  <x:si>
-    <x:t>황야 &lt;size=15&gt;부식성 바람 : 턴당 선체 내구도 - 1&lt;/size&gt;</x:t>
-  </x:si>
-  <x:si>
-    <x:t>이벤트(늪에 빠짐)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>지역 설명(사막)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>지역 설명(툰드라)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>게임 로드 문구</x:t>
-  </x:si>
-  <x:si>
-    <x:t>게임 나가기 문구</x:t>
-  </x:si>
-  <x:si>
-    <x:t>지역 설명(습지)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>게임 시작 문구</x:t>
-  </x:si>
-  <x:si>
-    <x:t>지역 설명(도시)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>JustoUda</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Japanese</x:t>
-  </x:si>
-  <x:si>
-    <x:t>이름(기획자용)</x:t>
+    <x:t>이벤트(수풀 속 길잃음)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>이벤트(사막 모래 폭풍)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>이벤트(툰드라 구조물 탐색)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STR_NOTE_SWAMP</x:t>
+  </x:si>
+  <x:si>
+    <x:t>알림(알림 사항 있음)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STR_WARNING_NOTICE_ALERT</x:t>
   </x:si>
   <x:si>
     <x:t>STR_OPTION_SCREEN_WINDOWED</x:t>
   </x:si>
   <x:si>
-    <x:t>STR_WARNING_NOTICE_ALERT</x:t>
-  </x:si>
-  <x:si>
     <x:t>경고 : 주변 1타일 이내에 글리처가 있습니다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>이벤트(툰드라 구조물 탐색)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>새로운 알림이 있습니다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>STR_NOTE_SWAMP</x:t>
-  </x:si>
-  <x:si>
-    <x:t>알림(알림 사항 있음)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>이벤트(수풀 속 길잃음)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>이벤트(도둑맞은 자원)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>이벤트(사막 모래 폭풍)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>STR_QUEST_MAIN_04</x:t>
-  </x:si>
-  <x:si>
-    <x:t>STR_QUEST_MAIN_01</x:t>
-  </x:si>
-  <x:si>
-    <x:t>STR_QUEST_MAIN_02</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -1411,7 +1411,7 @@
   <x:dimension ref="A1:H46"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" topLeftCell="A1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <x:selection activeCell="H44" activeCellId="0" sqref="C2:H44"/>
+      <x:selection activeCell="D30" activeCellId="0" sqref="D30:D30"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="16.399999999999999"/>
@@ -1426,67 +1426,67 @@
   <x:sheetData>
     <x:row r="1" spans="1:8">
       <x:c r="A1" s="14" t="s">
-        <x:v>51</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="B1" s="15" t="s">
-        <x:v>104</x:v>
+        <x:v>79</x:v>
       </x:c>
       <x:c r="C1" s="4" t="s">
-        <x:v>48</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="D1" s="4" t="s">
-        <x:v>47</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="E1" s="4" t="s">
-        <x:v>60</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="F1" s="7" t="s">
-        <x:v>49</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="G1" s="7" t="s">
-        <x:v>55</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="H1" s="7" t="s">
-        <x:v>59</x:v>
+        <x:v>52</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:8">
       <x:c r="A2" s="14"/>
       <x:c r="B2" s="15"/>
       <x:c r="C2" s="5" t="s">
-        <x:v>15</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="D2" s="5" t="s">
-        <x:v>12</x:v>
+        <x:v>90</x:v>
       </x:c>
       <x:c r="E2" s="5" t="s">
-        <x:v>7</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="F2" s="5" t="s">
-        <x:v>22</x:v>
+        <x:v>87</x:v>
       </x:c>
       <x:c r="G2" s="5" t="s">
-        <x:v>103</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="H2" s="5" t="s">
-        <x:v>6</x:v>
+        <x:v>101</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:8">
       <x:c r="A3" s="16" t="s">
-        <x:v>16</x:v>
+        <x:v>97</x:v>
       </x:c>
       <x:c r="B3" s="8" t="s">
-        <x:v>100</x:v>
+        <x:v>78</x:v>
       </x:c>
       <x:c r="C3" s="8">
         <x:v>1001</x:v>
       </x:c>
       <x:c r="D3" s="8" t="s">
-        <x:v>31</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="E3" s="8" t="s">
-        <x:v>20</x:v>
+        <x:v>91</x:v>
       </x:c>
       <x:c r="F3" s="8">
         <x:v>-1</x:v>
@@ -1501,16 +1501,16 @@
     <x:row r="4" spans="1:8">
       <x:c r="A4" s="17"/>
       <x:c r="B4" s="8" t="s">
-        <x:v>97</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="C4" s="8">
         <x:v>1002</x:v>
       </x:c>
       <x:c r="D4" s="8" t="s">
-        <x:v>76</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E4" s="8" t="s">
-        <x:v>8</x:v>
+        <x:v>102</x:v>
       </x:c>
       <x:c r="F4" s="8">
         <x:v>-1</x:v>
@@ -1525,16 +1525,16 @@
     <x:row r="5" spans="1:8">
       <x:c r="A5" s="17"/>
       <x:c r="B5" s="8" t="s">
-        <x:v>98</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="C5" s="8">
         <x:v>1003</x:v>
       </x:c>
       <x:c r="D5" s="8" t="s">
-        <x:v>65</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="E5" s="8" t="s">
-        <x:v>61</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="F5" s="8">
         <x:v>-1</x:v>
@@ -1549,16 +1549,16 @@
     <x:row r="6" spans="1:8">
       <x:c r="A6" s="17"/>
       <x:c r="B6" s="8" t="s">
-        <x:v>21</x:v>
+        <x:v>98</x:v>
       </x:c>
       <x:c r="C6" s="8">
         <x:v>1004</x:v>
       </x:c>
       <x:c r="D6" s="8" t="s">
-        <x:v>73</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="E6" s="8" t="s">
-        <x:v>9</x:v>
+        <x:v>103</x:v>
       </x:c>
       <x:c r="F6" s="8">
         <x:v>-1</x:v>
@@ -1573,16 +1573,16 @@
     <x:row r="7" spans="1:8">
       <x:c r="A7" s="17"/>
       <x:c r="B7" s="8" t="s">
-        <x:v>11</x:v>
+        <x:v>93</x:v>
       </x:c>
       <x:c r="C7" s="8">
         <x:v>1005</x:v>
       </x:c>
       <x:c r="D7" s="8" t="s">
-        <x:v>70</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="E7" s="8" t="s">
-        <x:v>10</x:v>
+        <x:v>104</x:v>
       </x:c>
       <x:c r="F7" s="8">
         <x:v>-1</x:v>
@@ -1597,16 +1597,16 @@
     <x:row r="8" spans="1:8">
       <x:c r="A8" s="18"/>
       <x:c r="B8" s="8" t="s">
-        <x:v>54</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="C8" s="8">
         <x:v>1006</x:v>
       </x:c>
       <x:c r="D8" s="8" t="s">
-        <x:v>66</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="E8" s="8" t="s">
-        <x:v>54</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="F8" s="8">
         <x:v>-1</x:v>
@@ -1621,16 +1621,16 @@
     <x:row r="9" spans="1:8">
       <x:c r="A9" s="6"/>
       <x:c r="B9" s="9" t="s">
-        <x:v>113</x:v>
+        <x:v>108</x:v>
       </x:c>
       <x:c r="C9" s="9">
         <x:v>2001</x:v>
       </x:c>
       <x:c r="D9" s="9" t="s">
-        <x:v>29</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="E9" s="9" t="s">
-        <x:v>23</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="F9" s="9">
         <x:v>-1</x:v>
@@ -1645,16 +1645,16 @@
     <x:row r="10" spans="1:8">
       <x:c r="A10" s="6"/>
       <x:c r="B10" s="9" t="s">
-        <x:v>114</x:v>
+        <x:v>111</x:v>
       </x:c>
       <x:c r="C10" s="9">
         <x:v>2002</x:v>
       </x:c>
       <x:c r="D10" s="9" t="s">
-        <x:v>38</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="E10" s="9" t="s">
-        <x:v>1</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="F10" s="9">
         <x:v>-1</x:v>
@@ -1669,7 +1669,7 @@
     <x:row r="11" spans="1:8" ht="32.75">
       <x:c r="A11" s="6"/>
       <x:c r="B11" s="9" t="s">
-        <x:v>108</x:v>
+        <x:v>112</x:v>
       </x:c>
       <x:c r="C11" s="9">
         <x:v>2003</x:v>
@@ -1678,7 +1678,7 @@
         <x:v>39</x:v>
       </x:c>
       <x:c r="E11" s="10" t="s">
-        <x:v>3</x:v>
+        <x:v>86</x:v>
       </x:c>
       <x:c r="F11" s="9">
         <x:v>-1</x:v>
@@ -1693,7 +1693,7 @@
     <x:row r="12" spans="1:8" ht="49.149999999999999">
       <x:c r="A12" s="6"/>
       <x:c r="B12" s="9" t="s">
-        <x:v>69</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="C12" s="9">
         <x:v>2004</x:v>
@@ -1702,7 +1702,7 @@
         <x:v>34</x:v>
       </x:c>
       <x:c r="E12" s="10" t="s">
-        <x:v>62</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="F12" s="9">
         <x:v>-1</x:v>
@@ -1717,16 +1717,16 @@
     <x:row r="13" spans="1:8" ht="49.149999999999999">
       <x:c r="A13" s="6"/>
       <x:c r="B13" s="9" t="s">
-        <x:v>112</x:v>
+        <x:v>110</x:v>
       </x:c>
       <x:c r="C13" s="9">
         <x:v>2005</x:v>
       </x:c>
       <x:c r="D13" s="9" t="s">
-        <x:v>71</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="E13" s="10" t="s">
-        <x:v>87</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="F13" s="9">
         <x:v>-1</x:v>
@@ -1741,13 +1741,13 @@
     <x:row r="14" spans="1:8" ht="32.75">
       <x:c r="A14" s="6"/>
       <x:c r="B14" s="9" t="s">
-        <x:v>94</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="C14" s="9">
         <x:v>2006</x:v>
       </x:c>
       <x:c r="D14" s="9" t="s">
-        <x:v>110</x:v>
+        <x:v>113</x:v>
       </x:c>
       <x:c r="E14" s="10" t="s">
         <x:v>2</x:v>
@@ -1765,16 +1765,16 @@
     <x:row r="15" spans="1:8">
       <x:c r="A15" s="6"/>
       <x:c r="B15" s="11" t="s">
-        <x:v>101</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="C15" s="11">
         <x:v>3001</x:v>
       </x:c>
       <x:c r="D15" s="11" t="s">
-        <x:v>75</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="E15" s="12" t="s">
-        <x:v>86</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="F15" s="11">
         <x:v>-1</x:v>
@@ -1789,16 +1789,16 @@
     <x:row r="16" spans="1:8">
       <x:c r="A16" s="6"/>
       <x:c r="B16" s="11" t="s">
-        <x:v>99</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="C16" s="11">
         <x:v>3002</x:v>
       </x:c>
       <x:c r="D16" s="11" t="s">
-        <x:v>26</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="E16" s="12" t="s">
-        <x:v>92</x:v>
+        <x:v>84</x:v>
       </x:c>
       <x:c r="F16" s="11">
         <x:v>-1</x:v>
@@ -1813,16 +1813,16 @@
     <x:row r="17" spans="1:8">
       <x:c r="A17" s="6"/>
       <x:c r="B17" s="11" t="s">
-        <x:v>95</x:v>
+        <x:v>73</x:v>
       </x:c>
       <x:c r="C17" s="11">
         <x:v>3003</x:v>
       </x:c>
       <x:c r="D17" s="11" t="s">
-        <x:v>35</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="E17" s="12" t="s">
-        <x:v>93</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="F17" s="11">
         <x:v>-1</x:v>
@@ -1837,16 +1837,16 @@
     <x:row r="18" spans="1:8">
       <x:c r="A18" s="6"/>
       <x:c r="B18" s="11" t="s">
-        <x:v>96</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="C18" s="11">
         <x:v>3004</x:v>
       </x:c>
       <x:c r="D18" s="11" t="s">
-        <x:v>30</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="E18" s="12" t="s">
-        <x:v>91</x:v>
+        <x:v>85</x:v>
       </x:c>
       <x:c r="F18" s="11">
         <x:v>-1</x:v>
@@ -1861,16 +1861,16 @@
     <x:row r="19" spans="1:8">
       <x:c r="A19" s="6"/>
       <x:c r="B19" s="13" t="s">
-        <x:v>111</x:v>
+        <x:v>114</x:v>
       </x:c>
       <x:c r="C19" s="13">
         <x:v>4001</x:v>
       </x:c>
       <x:c r="D19" s="13" t="s">
-        <x:v>36</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="E19" s="13" t="s">
-        <x:v>109</x:v>
+        <x:v>107</x:v>
       </x:c>
       <x:c r="F19" s="13">
         <x:v>-1</x:v>
@@ -1885,16 +1885,16 @@
     <x:row r="20" spans="1:8">
       <x:c r="A20" s="6"/>
       <x:c r="B20" s="13" t="s">
-        <x:v>63</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="C20" s="13">
         <x:v>4002</x:v>
       </x:c>
       <x:c r="D20" s="13" t="s">
-        <x:v>106</x:v>
+        <x:v>115</x:v>
       </x:c>
       <x:c r="E20" s="13" t="s">
-        <x:v>107</x:v>
+        <x:v>117</x:v>
       </x:c>
       <x:c r="F20" s="13">
         <x:v>-1</x:v>
@@ -1913,10 +1913,10 @@
         <x:v>5001</x:v>
       </x:c>
       <x:c r="D21" s="6" t="s">
-        <x:v>64</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="E21" s="6" t="s">
-        <x:v>56</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="F21" s="6">
         <x:v>-1</x:v>
@@ -1935,10 +1935,10 @@
         <x:v>5002</x:v>
       </x:c>
       <x:c r="D22" s="6" t="s">
-        <x:v>37</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="E22" s="6" t="s">
-        <x:v>13</x:v>
+        <x:v>89</x:v>
       </x:c>
       <x:c r="F22" s="6">
         <x:v>-1</x:v>
@@ -1957,10 +1957,10 @@
         <x:v>5003</x:v>
       </x:c>
       <x:c r="D23" s="6" t="s">
-        <x:v>28</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="E23" s="6" t="s">
-        <x:v>57</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="F23" s="6">
         <x:v>-1</x:v>
@@ -1979,10 +1979,10 @@
         <x:v>5004</x:v>
       </x:c>
       <x:c r="D24" s="6" t="s">
-        <x:v>33</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="E24" s="6" t="s">
-        <x:v>50</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="F24" s="6">
         <x:v>-1</x:v>
@@ -2001,10 +2001,10 @@
         <x:v>5005</x:v>
       </x:c>
       <x:c r="D25" s="6" t="s">
-        <x:v>68</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="E25" s="6" t="s">
-        <x:v>52</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="F25" s="6">
         <x:v>-1</x:v>
@@ -2023,10 +2023,10 @@
         <x:v>5006</x:v>
       </x:c>
       <x:c r="D26" s="6" t="s">
-        <x:v>90</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="E26" s="6" t="s">
-        <x:v>17</x:v>
+        <x:v>95</x:v>
       </x:c>
       <x:c r="F26" s="6">
         <x:v>-1</x:v>
@@ -2045,10 +2045,10 @@
         <x:v>5007</x:v>
       </x:c>
       <x:c r="D27" s="6" t="s">
-        <x:v>89</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="E27" s="6" t="s">
-        <x:v>18</x:v>
+        <x:v>92</x:v>
       </x:c>
       <x:c r="F27" s="6">
         <x:v>-1</x:v>
@@ -2067,10 +2067,10 @@
         <x:v>5008</x:v>
       </x:c>
       <x:c r="D28" s="6" t="s">
-        <x:v>105</x:v>
+        <x:v>116</x:v>
       </x:c>
       <x:c r="E28" s="6" t="s">
-        <x:v>19</x:v>
+        <x:v>99</x:v>
       </x:c>
       <x:c r="F28" s="6">
         <x:v>-1</x:v>
@@ -2089,10 +2089,10 @@
         <x:v>5009</x:v>
       </x:c>
       <x:c r="D29" s="6" t="s">
-        <x:v>88</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="E29" s="6" t="s">
-        <x:v>53</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="F29" s="6">
         <x:v>-1</x:v>
@@ -2111,10 +2111,10 @@
         <x:v>6001</x:v>
       </x:c>
       <x:c r="D30" s="6" t="s">
-        <x:v>72</x:v>
+        <x:v>105</x:v>
       </x:c>
       <x:c r="E30" s="6" t="s">
-        <x:v>27</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="F30" s="6">
         <x:v>-1</x:v>
@@ -2133,10 +2133,10 @@
         <x:v>6002</x:v>
       </x:c>
       <x:c r="D31" s="6" t="s">
-        <x:v>74</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="E31" s="6" t="s">
-        <x:v>67</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="F31" s="6">
         <x:v>-1</x:v>
@@ -2155,19 +2155,19 @@
         <x:v>7001</x:v>
       </x:c>
       <x:c r="D32" s="6" t="s">
-        <x:v>25</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="E32" s="6" t="s">
-        <x:v>102</x:v>
+        <x:v>75</x:v>
       </x:c>
       <x:c r="F32" s="6" t="s">
-        <x:v>102</x:v>
+        <x:v>75</x:v>
       </x:c>
       <x:c r="G32" s="6" t="s">
-        <x:v>102</x:v>
+        <x:v>75</x:v>
       </x:c>
       <x:c r="H32" s="6" t="s">
-        <x:v>102</x:v>
+        <x:v>75</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:8">
@@ -2177,13 +2177,13 @@
         <x:v>7002</x:v>
       </x:c>
       <x:c r="D33" s="6" t="s">
-        <x:v>32</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="E33" s="6" t="s">
-        <x:v>45</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="F33" s="6" t="s">
-        <x:v>14</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="G33" s="6">
         <x:v>-1</x:v>
@@ -2199,13 +2199,13 @@
         <x:v>7003</x:v>
       </x:c>
       <x:c r="D34" s="6" t="s">
-        <x:v>24</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="E34" s="6" t="s">
-        <x:v>58</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="F34" s="6" t="s">
-        <x:v>46</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="G34" s="6">
         <x:v>-1</x:v>
@@ -2221,10 +2221,10 @@
         <x:v>8001</x:v>
       </x:c>
       <x:c r="D35" s="6" t="s">
-        <x:v>40</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="E35" s="6" t="s">
-        <x:v>4</x:v>
+        <x:v>106</x:v>
       </x:c>
       <x:c r="F35" s="6">
         <x:v>-1</x:v>
@@ -2243,10 +2243,10 @@
         <x:v>8002</x:v>
       </x:c>
       <x:c r="D36" s="6" t="s">
-        <x:v>44</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="E36" s="6" t="s">
-        <x:v>85</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="F36" s="6">
         <x:v>-1</x:v>
@@ -2265,10 +2265,10 @@
         <x:v>8003</x:v>
       </x:c>
       <x:c r="D37" s="6" t="s">
-        <x:v>42</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="E37" s="6" t="s">
-        <x:v>5</x:v>
+        <x:v>109</x:v>
       </x:c>
       <x:c r="F37" s="6">
         <x:v>-1</x:v>
@@ -2285,10 +2285,10 @@
         <x:v>8004</x:v>
       </x:c>
       <x:c r="D38" s="6" t="s">
-        <x:v>41</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="E38" s="6" t="s">
-        <x:v>0</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="F38" s="6">
         <x:v>-1</x:v>
@@ -2308,7 +2308,7 @@
         <x:v>43</x:v>
       </x:c>
       <x:c r="E39" s="6" t="s">
-        <x:v>79</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="F39" s="6">
         <x:v>-1</x:v>
@@ -2325,10 +2325,10 @@
         <x:v>8006</x:v>
       </x:c>
       <x:c r="D40" s="6" t="s">
-        <x:v>116</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="E40" s="6" t="s">
-        <x:v>77</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="F40" s="6">
         <x:v>-1</x:v>
@@ -2345,10 +2345,10 @@
         <x:v>8007</x:v>
       </x:c>
       <x:c r="D41" s="6" t="s">
-        <x:v>117</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="E41" s="6" t="s">
-        <x:v>81</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="F41" s="6">
         <x:v>-1</x:v>
@@ -2365,10 +2365,10 @@
         <x:v>8008</x:v>
       </x:c>
       <x:c r="D42" s="6" t="s">
-        <x:v>82</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="E42" s="6" t="s">
-        <x:v>80</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="F42" s="6">
         <x:v>-1</x:v>
@@ -2385,10 +2385,10 @@
         <x:v>8009</x:v>
       </x:c>
       <x:c r="D43" s="6" t="s">
-        <x:v>115</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="E43" s="6" t="s">
-        <x:v>83</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="F43" s="6">
         <x:v>-1</x:v>
@@ -2405,10 +2405,10 @@
         <x:v>8010</x:v>
       </x:c>
       <x:c r="D44" s="6" t="s">
-        <x:v>84</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E44" s="6" t="s">
-        <x:v>78</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="F44" s="6">
         <x:v>-1</x:v>

</xml_diff>